<commit_message>
adding the python script to add new urls columns that will be used for cidoc modelization. updating the input excel file euterpe data
</commit_message>
<xml_diff>
--- a/input/taxonomies.xlsx
+++ b/input/taxonomies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cedric\Desktop\GIT\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A819D509-6E06-4AD5-84A7-397B0BC4AA29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E602F8E-8682-4E39-92B8-FCEFF4049F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spécialité" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11494" uniqueCount="11459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11503" uniqueCount="11463">
   <si>
     <t>name</t>
   </si>
@@ -34407,6 +34407,18 @@
   </si>
   <si>
     <t>301ceecd-ee25-498a-9db8-c9b176814bff</t>
+  </si>
+  <si>
+    <t>E55</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E53</t>
+  </si>
+  <si>
+    <t>E28</t>
   </si>
 </sst>
 </file>
@@ -34770,15 +34782,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -34788,8 +34800,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -34800,7 +34815,7 @@
         <v>7644</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -34811,7 +34826,7 @@
         <v>7645</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -34822,7 +34837,7 @@
         <v>7646</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -34833,7 +34848,7 @@
         <v>7647</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -34844,7 +34859,7 @@
         <v>7648</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -34855,7 +34870,7 @@
         <v>7649</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -34866,7 +34881,7 @@
         <v>7650</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -34877,7 +34892,7 @@
         <v>7651</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -34888,7 +34903,7 @@
         <v>7652</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -34899,7 +34914,7 @@
         <v>7653</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -34910,7 +34925,7 @@
         <v>7654</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -34921,7 +34936,7 @@
         <v>7655</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -34932,7 +34947,7 @@
         <v>7656</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -34943,7 +34958,7 @@
         <v>7657</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -35321,15 +35336,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -35339,8 +35354,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11460</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>56</v>
       </c>
@@ -35351,7 +35369,7 @@
         <v>7671</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>58</v>
       </c>
@@ -35362,7 +35380,7 @@
         <v>7672</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>60</v>
       </c>
@@ -35373,7 +35391,7 @@
         <v>7673</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>62</v>
       </c>
@@ -35384,7 +35402,7 @@
         <v>7674</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>64</v>
       </c>
@@ -35395,7 +35413,7 @@
         <v>7675</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
@@ -35406,7 +35424,7 @@
         <v>7676</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>68</v>
       </c>
@@ -35417,7 +35435,7 @@
         <v>7677</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -35428,7 +35446,7 @@
         <v>7678</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>72</v>
       </c>
@@ -35439,7 +35457,7 @@
         <v>7679</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>74</v>
       </c>
@@ -35450,7 +35468,7 @@
         <v>7680</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>76</v>
       </c>
@@ -35461,7 +35479,7 @@
         <v>7681</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>78</v>
       </c>
@@ -35472,7 +35490,7 @@
         <v>7682</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>80</v>
       </c>
@@ -35483,7 +35501,7 @@
         <v>7683</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
@@ -35494,7 +35512,7 @@
         <v>7684</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>84</v>
       </c>
@@ -35743,15 +35761,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -35761,8 +35779,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>128</v>
       </c>
@@ -35773,7 +35794,7 @@
         <v>7707</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>130</v>
       </c>
@@ -35784,7 +35805,7 @@
         <v>7708</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>132</v>
       </c>
@@ -35795,7 +35816,7 @@
         <v>7709</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>134</v>
       </c>
@@ -35806,7 +35827,7 @@
         <v>7710</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>136</v>
       </c>
@@ -35817,7 +35838,7 @@
         <v>7711</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>138</v>
       </c>
@@ -35828,7 +35849,7 @@
         <v>7712</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>140</v>
       </c>
@@ -35839,7 +35860,7 @@
         <v>7713</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>142</v>
       </c>
@@ -35850,7 +35871,7 @@
         <v>7714</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>144</v>
       </c>
@@ -35861,7 +35882,7 @@
         <v>7715</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>146</v>
       </c>
@@ -35872,7 +35893,7 @@
         <v>7716</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>148</v>
       </c>
@@ -35883,7 +35904,7 @@
         <v>7717</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>150</v>
       </c>
@@ -35894,7 +35915,7 @@
         <v>7718</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>152</v>
       </c>
@@ -35905,7 +35926,7 @@
         <v>7719</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>154</v>
       </c>
@@ -35916,7 +35937,7 @@
         <v>7720</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>156</v>
       </c>
@@ -36088,15 +36109,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -36106,8 +36127,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>227</v>
       </c>
@@ -36118,7 +36142,7 @@
         <v>7736</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>229</v>
       </c>
@@ -36129,7 +36153,7 @@
         <v>7737</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>231</v>
       </c>
@@ -36140,7 +36164,7 @@
         <v>7738</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>233</v>
       </c>
@@ -36151,7 +36175,7 @@
         <v>7739</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>235</v>
       </c>
@@ -36162,7 +36186,7 @@
         <v>7740</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>237</v>
       </c>
@@ -36173,7 +36197,7 @@
         <v>7741</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>239</v>
       </c>
@@ -36184,7 +36208,7 @@
         <v>7742</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>241</v>
       </c>
@@ -36195,7 +36219,7 @@
         <v>7743</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>243</v>
       </c>
@@ -36206,7 +36230,7 @@
         <v>7744</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>245</v>
       </c>
@@ -36217,7 +36241,7 @@
         <v>7745</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>247</v>
       </c>
@@ -36228,7 +36252,7 @@
         <v>7746</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>249</v>
       </c>
@@ -36239,7 +36263,7 @@
         <v>7747</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>251</v>
       </c>
@@ -36250,7 +36274,7 @@
         <v>7748</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>253</v>
       </c>
@@ -36261,7 +36285,7 @@
         <v>7749</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>255</v>
       </c>
@@ -36370,15 +36394,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D1350"/>
+  <dimension ref="A1:E1350"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1319" sqref="D1319"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -36388,8 +36412,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11461</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>273</v>
       </c>
@@ -36400,7 +36427,7 @@
         <v>7759</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>275</v>
       </c>
@@ -36411,7 +36438,7 @@
         <v>7760</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>277</v>
       </c>
@@ -36422,7 +36449,7 @@
         <v>7761</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>279</v>
       </c>
@@ -36433,7 +36460,7 @@
         <v>7762</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>281</v>
       </c>
@@ -36444,7 +36471,7 @@
         <v>7763</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>283</v>
       </c>
@@ -36455,7 +36482,7 @@
         <v>7764</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>285</v>
       </c>
@@ -36466,7 +36493,7 @@
         <v>7765</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>287</v>
       </c>
@@ -36477,7 +36504,7 @@
         <v>7766</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>289</v>
       </c>
@@ -36488,7 +36515,7 @@
         <v>7767</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>291</v>
       </c>
@@ -36499,7 +36526,7 @@
         <v>7768</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>293</v>
       </c>
@@ -36510,7 +36537,7 @@
         <v>7769</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>295</v>
       </c>
@@ -36521,7 +36548,7 @@
         <v>7770</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>297</v>
       </c>
@@ -36532,7 +36559,7 @@
         <v>7771</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>299</v>
       </c>
@@ -36543,7 +36570,7 @@
         <v>7772</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>301</v>
       </c>
@@ -51235,15 +51262,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D1882"/>
+  <dimension ref="A1:E1882"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -51253,8 +51280,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11462</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2950</v>
       </c>
@@ -51265,7 +51295,7 @@
         <v>9108</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2951</v>
       </c>
@@ -51276,7 +51306,7 @@
         <v>9109</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2953</v>
       </c>
@@ -51287,7 +51317,7 @@
         <v>9110</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2955</v>
       </c>
@@ -51298,7 +51328,7 @@
         <v>9111</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2957</v>
       </c>
@@ -51309,7 +51339,7 @@
         <v>9112</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2959</v>
       </c>
@@ -51320,7 +51350,7 @@
         <v>9113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2961</v>
       </c>
@@ -51331,7 +51361,7 @@
         <v>9114</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2963</v>
       </c>
@@ -51342,7 +51372,7 @@
         <v>9115</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2965</v>
       </c>
@@ -51353,7 +51383,7 @@
         <v>9116</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2967</v>
       </c>
@@ -51364,7 +51394,7 @@
         <v>9117</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2969</v>
       </c>
@@ -51375,7 +51405,7 @@
         <v>9118</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2971</v>
       </c>
@@ -51386,7 +51416,7 @@
         <v>9119</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>2973</v>
       </c>
@@ -51397,7 +51427,7 @@
         <v>9120</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2975</v>
       </c>
@@ -51408,7 +51438,7 @@
         <v>9121</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>2977</v>
       </c>
@@ -72000,15 +72030,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D495"/>
+  <dimension ref="A1:E495"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D398" sqref="D398"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -72018,8 +72048,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6712</v>
       </c>
@@ -72030,7 +72063,7 @@
         <v>10989</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6714</v>
       </c>
@@ -72041,7 +72074,7 @@
         <v>10990</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6716</v>
       </c>
@@ -72052,7 +72085,7 @@
         <v>10991</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>6718</v>
       </c>
@@ -72063,7 +72096,7 @@
         <v>10992</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6720</v>
       </c>
@@ -72074,7 +72107,7 @@
         <v>10993</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6722</v>
       </c>
@@ -72085,7 +72118,7 @@
         <v>10994</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>6724</v>
       </c>
@@ -72096,7 +72129,7 @@
         <v>10995</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>6726</v>
       </c>
@@ -72107,7 +72140,7 @@
         <v>10996</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>6728</v>
       </c>
@@ -72118,7 +72151,7 @@
         <v>10997</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>6730</v>
       </c>
@@ -72129,7 +72162,7 @@
         <v>10998</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>6732</v>
       </c>
@@ -72140,7 +72173,7 @@
         <v>10999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>6734</v>
       </c>
@@ -72151,7 +72184,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>6736</v>
       </c>
@@ -72162,7 +72195,7 @@
         <v>11001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>6738</v>
       </c>
@@ -72173,7 +72206,7 @@
         <v>11002</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>6740</v>
       </c>
@@ -76457,15 +76490,15 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -76475,8 +76508,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7516</v>
       </c>
@@ -76487,7 +76523,7 @@
         <v>11391</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7517</v>
       </c>
@@ -76498,7 +76534,7 @@
         <v>11392</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7519</v>
       </c>
@@ -76509,7 +76545,7 @@
         <v>11393</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7521</v>
       </c>
@@ -76520,7 +76556,7 @@
         <v>11394</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7523</v>
       </c>
@@ -76531,7 +76567,7 @@
         <v>11395</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7525</v>
       </c>
@@ -76542,7 +76578,7 @@
         <v>11396</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7527</v>
       </c>
@@ -76553,7 +76589,7 @@
         <v>11397</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7529</v>
       </c>
@@ -76564,7 +76600,7 @@
         <v>11398</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7531</v>
       </c>
@@ -76575,7 +76611,7 @@
         <v>11399</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7532</v>
       </c>
@@ -76586,7 +76622,7 @@
         <v>11400</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7533</v>
       </c>
@@ -76597,7 +76633,7 @@
         <v>11401</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7535</v>
       </c>
@@ -76608,7 +76644,7 @@
         <v>11402</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7537</v>
       </c>
@@ -76619,7 +76655,7 @@
         <v>11403</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7539</v>
       </c>
@@ -76630,7 +76666,7 @@
         <v>11404</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7541</v>
       </c>
@@ -76857,15 +76893,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -76875,8 +76911,11 @@
       <c r="D1" t="s">
         <v>7643</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>11459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7581</v>
       </c>
@@ -76887,7 +76926,7 @@
         <v>11425</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7583</v>
       </c>
@@ -76898,7 +76937,7 @@
         <v>11426</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>7585</v>
       </c>
@@ -76909,7 +76948,7 @@
         <v>11427</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>7587</v>
       </c>
@@ -76920,7 +76959,7 @@
         <v>11428</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>7589</v>
       </c>
@@ -76931,7 +76970,7 @@
         <v>11429</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7590</v>
       </c>
@@ -76942,7 +76981,7 @@
         <v>11430</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7592</v>
       </c>
@@ -76953,7 +76992,7 @@
         <v>11431</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>7594</v>
       </c>
@@ -76964,7 +77003,7 @@
         <v>11432</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>7595</v>
       </c>
@@ -76975,7 +77014,7 @@
         <v>11433</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>7597</v>
       </c>
@@ -76986,7 +77025,7 @@
         <v>11434</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7599</v>
       </c>
@@ -76997,7 +77036,7 @@
         <v>11435</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>7601</v>
       </c>
@@ -77008,7 +77047,7 @@
         <v>11436</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>7603</v>
       </c>
@@ -77019,7 +77058,7 @@
         <v>11437</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>7604</v>
       </c>
@@ -77030,7 +77069,7 @@
         <v>11438</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>7606</v>
       </c>

</xml_diff>